<commit_message>
china added indices und momentum chli gebastelt
</commit_message>
<xml_diff>
--- a/1_Data/Data Clean TM/Data_ETFxIndex_stiched.xlsx
+++ b/1_Data/Data Clean TM/Data_ETFxIndex_stiched.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Library/CloudStorage/Dropbox/00 UZH/Master/PMP/01. Offline PMP/PMP Coding/PMP-Term-Paper/1_Data/Data Clean TM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06810B0C-3CF9-DF42-8D0B-3C6B77F3E3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5806CB-0D92-5046-A4EB-C8F9C47E04CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="3160" windowWidth="26240" windowHeight="14740" xr2:uid="{E6F2891E-9DB8-E742-A471-87389AB6B4EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3157EA5A-40E7-AB45-90B4-60D15F0726B5}">
   <dimension ref="A1:N281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
+      <selection activeCell="H278" sqref="H278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5414,8 +5414,8 @@
       <c r="G113" s="2">
         <v>116.82905</v>
       </c>
-      <c r="H113" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H113" s="2">
+        <v>6.6109439079861003</v>
       </c>
       <c r="I113" s="2">
         <v>40.9423705287698</v>
@@ -5458,8 +5458,8 @@
       <c r="G114" s="2">
         <v>117.17005</v>
       </c>
-      <c r="H114" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H114" s="2">
+        <v>6.6243769275402267</v>
       </c>
       <c r="I114" s="2">
         <v>40.810626762424441</v>
@@ -5502,8 +5502,8 @@
       <c r="G115" s="2">
         <v>114.6824</v>
       </c>
-      <c r="H115" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H115" s="2">
+        <v>6.6734555652242413</v>
       </c>
       <c r="I115" s="2">
         <v>40.231609211636652</v>
@@ -5546,8 +5546,8 @@
       <c r="G116" s="2">
         <v>115.15039999999999</v>
       </c>
-      <c r="H116" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H116" s="2">
+        <v>6.6474595744875034</v>
       </c>
       <c r="I116" s="2">
         <v>39.938180874308983</v>
@@ -5590,8 +5590,8 @@
       <c r="G117" s="2">
         <v>112.24223333333333</v>
       </c>
-      <c r="H117" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H117" s="2">
+        <v>6.5277751932000534</v>
       </c>
       <c r="I117" s="2">
         <v>39.983440721544234</v>
@@ -5634,8 +5634,8 @@
       <c r="G118" s="2">
         <v>112.49076666666667</v>
       </c>
-      <c r="H118" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H118" s="2">
+        <v>6.5682126686488083</v>
       </c>
       <c r="I118" s="2">
         <v>40.280418850811913</v>
@@ -5678,8 +5678,8 @@
       <c r="G119" s="2">
         <v>112.69580000000001</v>
       </c>
-      <c r="H119" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H119" s="2">
+        <v>6.5793453330388578</v>
       </c>
       <c r="I119" s="2">
         <v>40.552717474210901</v>
@@ -5722,8 +5722,8 @@
       <c r="G120" s="2">
         <v>112.51299999999999</v>
       </c>
-      <c r="H120" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H120" s="2">
+        <v>6.5415048201535591</v>
       </c>
       <c r="I120" s="2">
         <v>40.453407818746072</v>
@@ -5766,8 +5766,8 @@
       <c r="G121" s="2">
         <v>114.03429999999999</v>
       </c>
-      <c r="H121" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H121" s="2">
+        <v>6.6107923086486391</v>
       </c>
       <c r="I121" s="2">
         <v>41.130340463879399</v>
@@ -5810,8 +5810,8 @@
       <c r="G122" s="2">
         <v>114.46903333333334</v>
       </c>
-      <c r="H122" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H122" s="2">
+        <v>6.6255963135154543</v>
       </c>
       <c r="I122" s="2">
         <v>40.858633472470416</v>
@@ -5854,8 +5854,8 @@
       <c r="G123" s="2">
         <v>114.3242</v>
       </c>
-      <c r="H123" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H123" s="2">
+        <v>6.642713856097429</v>
       </c>
       <c r="I123" s="2">
         <v>41.461865675420484</v>
@@ -5898,8 +5898,8 @@
       <c r="G124" s="2">
         <v>115.55883333333333</v>
       </c>
-      <c r="H124" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H124" s="2">
+        <v>6.7034656427659183</v>
       </c>
       <c r="I124" s="2">
         <v>41.641087908963605</v>
@@ -5942,8 +5942,8 @@
       <c r="G125" s="2">
         <v>114.99136666666668</v>
       </c>
-      <c r="H125" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H125" s="2">
+        <v>6.7563935853663271</v>
       </c>
       <c r="I125" s="2">
         <v>41.292130683431346</v>
@@ -5986,8 +5986,8 @@
       <c r="G126" s="2">
         <v>115.27640000000001</v>
       </c>
-      <c r="H126" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H126" s="2">
+        <v>6.7918941954342973</v>
       </c>
       <c r="I126" s="2">
         <v>41.520162556149728</v>
@@ -6030,8 +6030,8 @@
       <c r="G127" s="2">
         <v>116.97446666666667</v>
       </c>
-      <c r="H127" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H127" s="2">
+        <v>6.843655482263812</v>
       </c>
       <c r="I127" s="2">
         <v>42.324127041422315</v>
@@ -6074,8 +6074,8 @@
       <c r="G128" s="2">
         <v>117.8326</v>
       </c>
-      <c r="H128" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H128" s="2">
+        <v>6.8907501460097551</v>
       </c>
       <c r="I128" s="2">
         <v>42.964209465464016</v>
@@ -6118,8 +6118,8 @@
       <c r="G129" s="2">
         <v>117.5964</v>
       </c>
-      <c r="H129" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H129" s="2">
+        <v>6.9251038741334581</v>
       </c>
       <c r="I129" s="2">
         <v>43.005074332202092</v>
@@ -6162,8 +6162,8 @@
       <c r="G130" s="2">
         <v>119.04063333333333</v>
       </c>
-      <c r="H130" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H130" s="2">
+        <v>6.9247149888764934</v>
       </c>
       <c r="I130" s="2">
         <v>43.93165454740285</v>
@@ -6206,8 +6206,8 @@
       <c r="G131" s="2">
         <v>118.34216666666667</v>
       </c>
-      <c r="H131" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H131" s="2">
+        <v>7.025541730838941</v>
       </c>
       <c r="I131" s="2">
         <v>43.495178046777973</v>
@@ -6250,8 +6250,8 @@
       <c r="G132" s="2">
         <v>117.7471</v>
       </c>
-      <c r="H132" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H132" s="2">
+        <v>6.9441197040714631</v>
       </c>
       <c r="I132" s="2">
         <v>43.383232822383796</v>
@@ -6294,8 +6294,8 @@
       <c r="G133" s="2">
         <v>117.73509999999999</v>
       </c>
-      <c r="H133" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H133" s="2">
+        <v>6.7989600428150734</v>
       </c>
       <c r="I133" s="2">
         <v>43.253475249147733</v>
@@ -6338,8 +6338,8 @@
       <c r="G134" s="2">
         <v>116.92626666666666</v>
       </c>
-      <c r="H134" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H134" s="2">
+        <v>6.9377854882758223</v>
       </c>
       <c r="I134" s="2">
         <v>43.216350341775026</v>
@@ -6382,8 +6382,8 @@
       <c r="G135" s="2">
         <v>116.38116666666667</v>
       </c>
-      <c r="H135" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H135" s="2">
+        <v>6.9257300453099262</v>
       </c>
       <c r="I135" s="2">
         <v>43.592290211994211</v>
@@ -6426,8 +6426,8 @@
       <c r="G136" s="2">
         <v>116.25563333333332</v>
       </c>
-      <c r="H136" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H136" s="2">
+        <v>6.9738595393159271</v>
       </c>
       <c r="I136" s="2">
         <v>43.777259727725934</v>
@@ -6470,8 +6470,8 @@
       <c r="G137" s="2">
         <v>116.03016666666667</v>
       </c>
-      <c r="H137" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H137" s="2">
+        <v>7.0570084802753481</v>
       </c>
       <c r="I137" s="2">
         <v>44.055136595602093</v>
@@ -6514,8 +6514,8 @@
       <c r="G138" s="2">
         <v>115.28773333333334</v>
       </c>
-      <c r="H138" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H138" s="2">
+        <v>7.1551855294700051</v>
       </c>
       <c r="I138" s="2">
         <v>44.273258632487916</v>
@@ -6558,8 +6558,8 @@
       <c r="G139" s="2">
         <v>117.24056666666667</v>
       </c>
-      <c r="H139" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H139" s="2">
+        <v>7.198411114472929</v>
       </c>
       <c r="I139" s="2">
         <v>44.872856524642252</v>
@@ -6602,8 +6602,8 @@
       <c r="G140" s="2">
         <v>118.14846666666665</v>
       </c>
-      <c r="H140" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H140" s="2">
+        <v>7.1771872072284308</v>
       </c>
       <c r="I140" s="2">
         <v>45.121257441587879</v>
@@ -6646,8 +6646,8 @@
       <c r="G141" s="2">
         <v>120.30943333333335</v>
       </c>
-      <c r="H141" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H141" s="2">
+        <v>7.1527533487950921</v>
       </c>
       <c r="I141" s="2">
         <v>45.956895368039575</v>
@@ -6690,8 +6690,8 @@
       <c r="G142" s="2">
         <v>121.37309999999998</v>
       </c>
-      <c r="H142" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H142" s="2">
+        <v>7.2057603867020017</v>
       </c>
       <c r="I142" s="2">
         <v>46.983672686690163</v>
@@ -6734,8 +6734,8 @@
       <c r="G143" s="2">
         <v>122.34310000000001</v>
       </c>
-      <c r="H143" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H143" s="2">
+        <v>7.3160390177913461</v>
       </c>
       <c r="I143" s="2">
         <v>47.455118863867007</v>
@@ -6778,8 +6778,8 @@
       <c r="G144" s="2">
         <v>122.1818</v>
       </c>
-      <c r="H144" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H144" s="2">
+        <v>7.4507449160384889</v>
       </c>
       <c r="I144" s="2">
         <v>47.106077119479039</v>
@@ -6822,8 +6822,8 @@
       <c r="G145" s="2">
         <v>123.22580000000001</v>
       </c>
-      <c r="H145" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H145" s="2">
+        <v>7.5387977660009868</v>
       </c>
       <c r="I145" s="2">
         <v>48.276937957409338</v>
@@ -6866,8 +6866,8 @@
       <c r="G146" s="2">
         <v>124.18490000000001</v>
       </c>
-      <c r="H146" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H146" s="2">
+        <v>7.741367437226188</v>
       </c>
       <c r="I146" s="2">
         <v>48.667393941097529</v>
@@ -6910,8 +6910,8 @@
       <c r="G147" s="2">
         <v>123.93043333333333</v>
       </c>
-      <c r="H147" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H147" s="2">
+        <v>7.746455901944433</v>
       </c>
       <c r="I147" s="2">
         <v>48.584523203069224</v>
@@ -6954,8 +6954,8 @@
       <c r="G148" s="2">
         <v>124.36733333333332</v>
       </c>
-      <c r="H148" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H148" s="2">
+        <v>7.7343345462231197</v>
       </c>
       <c r="I148" s="2">
         <v>48.380008701953464</v>
@@ -6998,8 +6998,8 @@
       <c r="G149" s="2">
         <v>123.39386666666667</v>
       </c>
-      <c r="H149" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H149" s="2">
+        <v>7.7852719236099146</v>
       </c>
       <c r="I149" s="2">
         <v>48.728395425209648</v>
@@ -7042,8 +7042,8 @@
       <c r="G150" s="2">
         <v>124.15593333333334</v>
       </c>
-      <c r="H150" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H150" s="2">
+        <v>7.7574962884768972</v>
       </c>
       <c r="I150" s="2">
         <v>50.1</v>
@@ -7086,8 +7086,8 @@
       <c r="G151" s="2">
         <v>125.2221</v>
       </c>
-      <c r="H151" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H151" s="2">
+        <v>7.8283261354487523</v>
       </c>
       <c r="I151" s="2">
         <v>51.2</v>
@@ -7130,8 +7130,8 @@
       <c r="G152" s="2">
         <v>124.61399999999999</v>
       </c>
-      <c r="H152" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H152" s="2">
+        <v>7.8709453231018331</v>
       </c>
       <c r="I152" s="2">
         <v>51.65</v>
@@ -7174,8 +7174,8 @@
       <c r="G153" s="2">
         <v>125.88356666666668</v>
       </c>
-      <c r="H153" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H153" s="2">
+        <v>7.8943904902039082</v>
       </c>
       <c r="I153" s="2">
         <v>51.758899999999997</v>
@@ -7218,8 +7218,8 @@
       <c r="G154" s="2">
         <v>125.66126666666666</v>
       </c>
-      <c r="H154" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H154" s="2">
+        <v>7.8603926909594604</v>
       </c>
       <c r="I154" s="2">
         <v>51.5852</v>
@@ -7262,8 +7262,8 @@
       <c r="G155" s="2">
         <v>124.99296666666667</v>
       </c>
-      <c r="H155" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H155" s="2">
+        <v>7.9228384354421841</v>
       </c>
       <c r="I155" s="2">
         <v>52.423099999999998</v>
@@ -7306,8 +7306,8 @@
       <c r="G156" s="2">
         <v>125.24510000000002</v>
       </c>
-      <c r="H156" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H156" s="2">
+        <v>7.9705592703645953</v>
       </c>
       <c r="I156" s="2">
         <v>52.312399999999997</v>
@@ -7350,8 +7350,8 @@
       <c r="G157" s="2">
         <v>125.66723333333334</v>
       </c>
-      <c r="H157" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H157" s="2">
+        <v>8.0201718013674945</v>
       </c>
       <c r="I157" s="2">
         <v>52.281300000000002</v>
@@ -7394,8 +7394,8 @@
       <c r="G158" s="2">
         <v>125.63276666666667</v>
       </c>
-      <c r="H158" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H158" s="2">
+        <v>8.0337168726058312</v>
       </c>
       <c r="I158" s="2">
         <v>52.177599999999998</v>
@@ -7438,8 +7438,8 @@
       <c r="G159" s="2">
         <v>123.92706666666668</v>
       </c>
-      <c r="H159" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H159" s="2">
+        <v>8.0639774186180944</v>
       </c>
       <c r="I159" s="2">
         <v>52.130600000000001</v>
@@ -7482,8 +7482,8 @@
       <c r="G160" s="2">
         <v>124.59236666666668</v>
       </c>
-      <c r="H160" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H160" s="2">
+        <v>8.0870205179121211</v>
       </c>
       <c r="I160" s="2">
         <v>52.415599999999998</v>
@@ -7526,8 +7526,8 @@
       <c r="G161" s="2">
         <v>124.50043333333333</v>
       </c>
-      <c r="H161" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H161" s="2">
+        <v>8.1209853607788585</v>
       </c>
       <c r="I161" s="2">
         <v>52.394500000000001</v>
@@ -7570,8 +7570,8 @@
       <c r="G162" s="2">
         <v>125.31696666666666</v>
       </c>
-      <c r="H162" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H162" s="2">
+        <v>8.2534765904439649</v>
       </c>
       <c r="I162" s="2">
         <v>53.121000000000002</v>
@@ -7614,8 +7614,8 @@
       <c r="G163" s="2">
         <v>124.37909999999999</v>
       </c>
-      <c r="H163" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H163" s="2">
+        <v>8.3235945796573088</v>
       </c>
       <c r="I163" s="2">
         <v>52.937100000000001</v>
@@ -7658,8 +7658,8 @@
       <c r="G164" s="2">
         <v>122.62150000000001</v>
       </c>
-      <c r="H164" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H164" s="2">
+        <v>8.3043612376264271</v>
       </c>
       <c r="I164" s="2">
         <v>52.320599999999999</v>
@@ -7702,8 +7702,8 @@
       <c r="G165" s="2">
         <v>122.97853333333335</v>
       </c>
-      <c r="H165" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H165" s="2">
+        <v>8.2466150726049836</v>
       </c>
       <c r="I165" s="2">
         <v>52.736600000000003</v>
@@ -7746,8 +7746,8 @@
       <c r="G166" s="2">
         <v>122.54129999999999</v>
       </c>
-      <c r="H166" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H166" s="2">
+        <v>8.1463222239614197</v>
       </c>
       <c r="I166" s="2">
         <v>52.580100000000002</v>
@@ -7790,8 +7790,8 @@
       <c r="G167" s="2">
         <v>122.79753333333333</v>
       </c>
-      <c r="H167" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H167" s="2">
+        <v>8.1372789939181125</v>
       </c>
       <c r="I167" s="2">
         <v>52.770099999999999</v>
@@ -7834,8 +7834,8 @@
       <c r="G168" s="2">
         <v>123.36226666666666</v>
       </c>
-      <c r="H168" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H168" s="2">
+        <v>8.1304965713856312</v>
       </c>
       <c r="I168" s="2">
         <v>52.817799999999998</v>
@@ -7878,8 +7878,8 @@
       <c r="G169" s="2">
         <v>123.86449999999998</v>
       </c>
-      <c r="H169" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H169" s="2">
+        <v>8.0400840447791797</v>
       </c>
       <c r="I169" s="2">
         <v>52.716000000000001</v>
@@ -7922,8 +7922,8 @@
       <c r="G170" s="2">
         <v>122.50846666666666</v>
       </c>
-      <c r="H170" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H170" s="2">
+        <v>8.0562524436831406</v>
       </c>
       <c r="I170" s="2">
         <v>52.942100000000003</v>
@@ -7966,8 +7966,8 @@
       <c r="G171" s="2">
         <v>124.37083333333332</v>
       </c>
-      <c r="H171" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H171" s="2">
+        <v>8.1630640638375151</v>
       </c>
       <c r="I171" s="2">
         <v>53.566400000000002</v>
@@ -8010,8 +8010,8 @@
       <c r="G172" s="2">
         <v>124.06919999999998</v>
       </c>
-      <c r="H172" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H172" s="2">
+        <v>8.1441009641038438</v>
       </c>
       <c r="I172" s="2">
         <v>53.692</v>
@@ -8054,8 +8054,8 @@
       <c r="G173" s="2">
         <v>124.31076666666668</v>
       </c>
-      <c r="H173" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H173" s="2">
+        <v>8.0420943838194194</v>
       </c>
       <c r="I173" s="2">
         <v>53.749200000000002</v>
@@ -8098,8 +8098,8 @@
       <c r="G174" s="2">
         <v>124.77816666666666</v>
       </c>
-      <c r="H174" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H174" s="2">
+        <v>8.055883332252801</v>
       </c>
       <c r="I174" s="2">
         <v>54.0914</v>
@@ -8142,8 +8142,8 @@
       <c r="G175" s="2">
         <v>125.444</v>
       </c>
-      <c r="H175" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H175" s="2">
+        <v>8.1986569517630699</v>
       </c>
       <c r="I175" s="2">
         <v>55.043900000000001</v>
@@ -8186,8 +8186,8 @@
       <c r="G176" s="2">
         <v>125.81610000000001</v>
       </c>
-      <c r="H176" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H176" s="2">
+        <v>8.3227311225613381</v>
       </c>
       <c r="I176" s="2">
         <v>55.601399999999998</v>
@@ -8230,8 +8230,8 @@
       <c r="G177" s="2">
         <v>126.27659999999999</v>
       </c>
-      <c r="H177" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H177" s="2">
+        <v>8.3072745814158893</v>
       </c>
       <c r="I177" s="2">
         <v>55.700200000000002</v>
@@ -8274,8 +8274,8 @@
       <c r="G178" s="2">
         <v>126.79773333333333</v>
       </c>
-      <c r="H178" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H178" s="2">
+        <v>8.3833774488211574</v>
       </c>
       <c r="I178" s="2">
         <v>56.278500000000001</v>
@@ -8318,8 +8318,8 @@
       <c r="G179" s="2">
         <v>126.831</v>
       </c>
-      <c r="H179" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H179" s="2">
+        <v>8.4969649002324701</v>
       </c>
       <c r="I179" s="2">
         <v>56.101500000000001</v>
@@ -8362,8 +8362,8 @@
       <c r="G180" s="2">
         <v>126.88573333333333</v>
       </c>
-      <c r="H180" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H180" s="2">
+        <v>8.7062181248570258</v>
       </c>
       <c r="I180" s="2">
         <v>56.595199999999998</v>
@@ -8406,8 +8406,8 @@
       <c r="G181" s="2">
         <v>127.9033</v>
       </c>
-      <c r="H181" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H181" s="2">
+        <v>8.8106700683674468</v>
       </c>
       <c r="I181" s="2">
         <v>57.380099999999999</v>
@@ -8450,8 +8450,8 @@
       <c r="G182" s="2">
         <v>128.46716666666669</v>
       </c>
-      <c r="H182" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H182" s="2">
+        <v>8.6882898553834131</v>
       </c>
       <c r="I182" s="2">
         <v>58.462299999999999</v>
@@ -8494,8 +8494,8 @@
       <c r="G183" s="2">
         <v>131.9127</v>
       </c>
-      <c r="H183" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H183" s="2">
+        <v>8.7037332139777792</v>
       </c>
       <c r="I183" s="2">
         <v>59.470500000000001</v>
@@ -8538,8 +8538,8 @@
       <c r="G184" s="2">
         <v>130.91373333333334</v>
       </c>
-      <c r="H184" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H184" s="2">
+        <v>8.8042369834386793</v>
       </c>
       <c r="I184" s="2">
         <v>59.590299999999999</v>
@@ -8582,8 +8582,8 @@
       <c r="G185" s="2">
         <v>131.46086666666667</v>
       </c>
-      <c r="H185" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H185" s="2">
+        <v>8.8149214410918884</v>
       </c>
       <c r="I185" s="2">
         <v>60.021299999999997</v>
@@ -8626,8 +8626,8 @@
       <c r="G186" s="2">
         <v>130.94516666666667</v>
       </c>
-      <c r="H186" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H186" s="2">
+        <v>8.9032445333516002</v>
       </c>
       <c r="I186" s="2">
         <v>59.365299999999998</v>
@@ -8670,8 +8670,8 @@
       <c r="G187" s="2">
         <v>131.66086666666664</v>
       </c>
-      <c r="H187" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H187" s="2">
+        <v>8.9121427553329884</v>
       </c>
       <c r="I187" s="2">
         <v>59.027999999999999</v>
@@ -8714,8 +8714,8 @@
       <c r="G188" s="2">
         <v>130.38310000000001</v>
       </c>
-      <c r="H188" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H188" s="2">
+        <v>8.9544191966578968</v>
       </c>
       <c r="I188" s="2">
         <v>58.750799999999998</v>
@@ -8758,8 +8758,8 @@
       <c r="G189" s="2">
         <v>130.91026666666667</v>
       </c>
-      <c r="H189" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H189" s="2">
+        <v>9.0084676561004056</v>
       </c>
       <c r="I189" s="2">
         <v>59.469299999999997</v>
@@ -8802,8 +8802,8 @@
       <c r="G190" s="2">
         <v>131.41423333333333</v>
       </c>
-      <c r="H190" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H190" s="2">
+        <v>8.8146577900702177</v>
       </c>
       <c r="I190" s="2">
         <v>59.821100000000001</v>
@@ -8846,8 +8846,8 @@
       <c r="G191" s="2">
         <v>131.60130000000001</v>
       </c>
-      <c r="H191" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H191" s="2">
+        <v>8.9167764220388523</v>
       </c>
       <c r="I191" s="2">
         <v>60.0032</v>
@@ -8890,8 +8890,8 @@
       <c r="G192" s="2">
         <v>132.45866666666666</v>
       </c>
-      <c r="H192" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H192" s="2">
+        <v>9.0807805400691599</v>
       </c>
       <c r="I192" s="2">
         <v>60.161900000000003</v>
@@ -8934,8 +8934,8 @@
       <c r="G193" s="2">
         <v>133.52119999999999</v>
       </c>
-      <c r="H193" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H193" s="2">
+        <v>8.9818520854627426</v>
       </c>
       <c r="I193" s="2">
         <v>59.417400000000001</v>
@@ -8978,8 +8978,8 @@
       <c r="G194" s="2">
         <v>131.16823333333332</v>
       </c>
-      <c r="H194" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H194" s="2">
+        <v>9.008566525233535</v>
       </c>
       <c r="I194" s="2">
         <v>59.710299999999997</v>
@@ -9022,8 +9022,8 @@
       <c r="G195" s="2">
         <v>132.62043333333335</v>
       </c>
-      <c r="H195" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H195" s="2">
+        <v>8.9124261801812832</v>
       </c>
       <c r="I195" s="2">
         <v>60.4985</v>
@@ -9066,8 +9066,8 @@
       <c r="G196" s="2">
         <v>134.1138</v>
       </c>
-      <c r="H196" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H196" s="2">
+        <v>8.96668556044113</v>
       </c>
       <c r="I196" s="2">
         <v>61.309199999999997</v>
@@ -9110,8 +9110,8 @@
       <c r="G197" s="2">
         <v>133.03836666666666</v>
       </c>
-      <c r="H197" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H197" s="2">
+        <v>9.1494089010100641</v>
       </c>
       <c r="I197" s="2">
         <v>61.112699999999997</v>
@@ -9154,8 +9154,8 @@
       <c r="G198" s="2">
         <v>132.0984</v>
       </c>
-      <c r="H198" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H198" s="2">
+        <v>9.0859349175428239</v>
       </c>
       <c r="I198" s="2">
         <v>61.4358</v>
@@ -9198,8 +9198,8 @@
       <c r="G199" s="2">
         <v>132.60496666666668</v>
       </c>
-      <c r="H199" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H199" s="2">
+        <v>8.9612148017414626</v>
       </c>
       <c r="I199" s="2">
         <v>61.880899999999997</v>
@@ -9242,8 +9242,8 @@
       <c r="G200" s="2">
         <v>134.87503333333333</v>
       </c>
-      <c r="H200" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H200" s="2">
+        <v>8.9240400076858819</v>
       </c>
       <c r="I200" s="2">
         <v>62.758800000000001</v>
@@ -9286,8 +9286,8 @@
       <c r="G201" s="2">
         <v>134.21076666666667</v>
       </c>
-      <c r="H201" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H201" s="2">
+        <v>8.953035028794126</v>
       </c>
       <c r="I201" s="2">
         <v>63.387</v>
@@ -9330,8 +9330,8 @@
       <c r="G202" s="2">
         <v>133.19353333333333</v>
       </c>
-      <c r="H202" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H202" s="2">
+        <v>8.9978161548249069</v>
       </c>
       <c r="I202" s="2">
         <v>63.561100000000003</v>
@@ -9374,8 +9374,8 @@
       <c r="G203" s="2">
         <v>133.88283333333334</v>
       </c>
-      <c r="H203" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H203" s="2">
+        <v>9.0374824510352756</v>
       </c>
       <c r="I203" s="2">
         <v>63.436700000000002</v>
@@ -9418,8 +9418,8 @@
       <c r="G204" s="2">
         <v>132.52806666666666</v>
       </c>
-      <c r="H204" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H204" s="2">
+        <v>8.9643852052770541</v>
       </c>
       <c r="I204" s="2">
         <v>62.489600000000003</v>
@@ -9462,8 +9462,8 @@
       <c r="G205" s="2">
         <v>130.90009999999998</v>
       </c>
-      <c r="H205" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H205" s="2">
+        <v>8.7252735024482835</v>
       </c>
       <c r="I205" s="2">
         <v>61.300899999999999</v>
@@ -9506,8 +9506,8 @@
       <c r="G206" s="2">
         <v>131.14243333333334</v>
       </c>
-      <c r="H206" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H206" s="2">
+        <v>8.5941071191670702</v>
       </c>
       <c r="I206" s="2">
         <v>61.288400000000003</v>
@@ -9550,8 +9550,8 @@
       <c r="G207" s="2">
         <v>130.471</v>
       </c>
-      <c r="H207" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H207" s="2">
+        <v>8.5991889926097738</v>
       </c>
       <c r="I207" s="2">
         <v>61.649799999999999</v>
@@ -9594,8 +9594,8 @@
       <c r="G208" s="2">
         <v>131.60766666666666</v>
       </c>
-      <c r="H208" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H208" s="2">
+        <v>8.6220409449130884</v>
       </c>
       <c r="I208" s="2">
         <v>61.712800000000001</v>
@@ -9638,8 +9638,8 @@
       <c r="G209" s="2">
         <v>130.64103333333333</v>
       </c>
-      <c r="H209" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H209" s="2">
+        <v>8.6103677959286156</v>
       </c>
       <c r="I209" s="2">
         <v>61.927100000000003</v>
@@ -9682,8 +9682,8 @@
       <c r="G210" s="2">
         <v>130.5701</v>
       </c>
-      <c r="H210" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H210" s="2">
+        <v>8.5451273506161805</v>
       </c>
       <c r="I210" s="2">
         <v>62.402700000000003</v>
@@ -9726,8 +9726,8 @@
       <c r="G211" s="2">
         <v>131.22209999999998</v>
       </c>
-      <c r="H211" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H211" s="2">
+        <v>8.5960119977986409</v>
       </c>
       <c r="I211" s="2">
         <v>63.201599999999999</v>
@@ -9770,8 +9770,8 @@
       <c r="G212" s="2">
         <v>130.10343333333333</v>
       </c>
-      <c r="H212" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H212" s="2">
+        <v>8.6796289193215301</v>
       </c>
       <c r="I212" s="2">
         <v>62.630899999999997</v>
@@ -9814,8 +9814,8 @@
       <c r="G213" s="2">
         <v>129.46296666666669</v>
       </c>
-      <c r="H213" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H213" s="2">
+        <v>8.7585660352097605</v>
       </c>
       <c r="I213" s="2">
         <v>62.5548</v>
@@ -9858,8 +9858,8 @@
       <c r="G214" s="2">
         <v>130.78229999999999</v>
       </c>
-      <c r="H214" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H214" s="2">
+        <v>8.9127161963051211</v>
       </c>
       <c r="I214" s="2">
         <v>62.631399999999999</v>
@@ -9902,8 +9902,8 @@
       <c r="G215" s="2">
         <v>129.72483333333335</v>
       </c>
-      <c r="H215" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H215" s="2">
+        <v>8.8855799148996564</v>
       </c>
       <c r="I215" s="2">
         <v>62.363199999999999</v>
@@ -9946,8 +9946,8 @@
       <c r="G216" s="2">
         <v>130.13496666666666</v>
       </c>
-      <c r="H216" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H216" s="2">
+        <v>8.8145589209370918</v>
       </c>
       <c r="I216" s="2">
         <v>63.015300000000003</v>
@@ -9990,8 +9990,8 @@
       <c r="G217" s="2">
         <v>130.04323333333335</v>
       </c>
-      <c r="H217" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H217" s="2">
+        <v>8.8886975882309152</v>
       </c>
       <c r="I217" s="2">
         <v>63.695799999999998</v>
@@ -10034,8 +10034,8 @@
       <c r="G218" s="2">
         <v>130.09959999999998</v>
       </c>
-      <c r="H218" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H218" s="2">
+        <v>9.0477252932271863</v>
       </c>
       <c r="I218" s="2">
         <v>63.169400000000003</v>
@@ -10078,8 +10078,8 @@
       <c r="G219" s="2">
         <v>129.16426666666666</v>
       </c>
-      <c r="H219" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H219" s="2">
+        <v>9.3922446745199348</v>
       </c>
       <c r="I219" s="2">
         <v>62.994100000000003</v>
@@ -10122,8 +10122,8 @@
       <c r="G220" s="2">
         <v>129.49189999999999</v>
       </c>
-      <c r="H220" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H220" s="2">
+        <v>9.4236850588541756</v>
       </c>
       <c r="I220" s="2">
         <v>63.1751</v>
@@ -10166,8 +10166,8 @@
       <c r="G221" s="2">
         <v>129.6806</v>
       </c>
-      <c r="H221" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H221" s="2">
+        <v>9.5336209436153467</v>
       </c>
       <c r="I221" s="2">
         <v>63.834699999999998</v>
@@ -10210,8 +10210,8 @@
       <c r="G222" s="2">
         <v>129.292</v>
       </c>
-      <c r="H222" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H222" s="2">
+        <v>9.5936015510454506</v>
       </c>
       <c r="I222" s="2">
         <v>63.3782</v>
@@ -10254,8 +10254,8 @@
       <c r="G223" s="2">
         <v>130.06553333333332</v>
       </c>
-      <c r="H223" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H223" s="2">
+        <v>9.533752769126183</v>
       </c>
       <c r="I223" s="2">
         <v>63.952800000000003</v>
@@ -10298,8 +10298,8 @@
       <c r="G224" s="2">
         <v>129.78886666666668</v>
       </c>
-      <c r="H224" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H224" s="2">
+        <v>9.2556866278455541</v>
       </c>
       <c r="I224" s="2">
         <v>64.253200000000007</v>
@@ -10342,8 +10342,8 @@
       <c r="G225" s="2">
         <v>129.02933333333331</v>
       </c>
-      <c r="H225" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H225" s="2">
+        <v>9.0512845820197416</v>
       </c>
       <c r="I225" s="2">
         <v>64.358000000000004</v>
@@ -10386,8 +10386,8 @@
       <c r="G226" s="2">
         <v>129.86323333333334</v>
       </c>
-      <c r="H226" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H226" s="2">
+        <v>9.0273318867009511</v>
       </c>
       <c r="I226" s="2">
         <v>64.909800000000004</v>
@@ -10430,8 +10430,8 @@
       <c r="G227" s="2">
         <v>128.72403333333332</v>
       </c>
-      <c r="H227" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H227" s="2">
+        <v>8.9587892123420918</v>
       </c>
       <c r="I227" s="2">
         <v>64.541899999999998</v>
@@ -10474,8 +10474,8 @@
       <c r="G228" s="2">
         <v>129.11043333333333</v>
       </c>
-      <c r="H228" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H228" s="2">
+        <v>8.9304928664412735</v>
       </c>
       <c r="I228" s="2">
         <v>65.031499999999994</v>
@@ -10518,8 +10518,8 @@
       <c r="G229" s="2">
         <v>129.80600000000001</v>
       </c>
-      <c r="H229" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H229" s="2">
+        <v>9.0841816382487135</v>
       </c>
       <c r="I229" s="2">
         <v>65.031499999999994</v>
@@ -10562,8 +10562,8 @@
       <c r="G230" s="2">
         <v>130.80043333333333</v>
       </c>
-      <c r="H230" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H230" s="2">
+        <v>9.2846289187494637</v>
       </c>
       <c r="I230" s="2">
         <v>66.100999999999999</v>
@@ -10606,8 +10606,8 @@
       <c r="G231" s="2">
         <v>131.23043333333331</v>
       </c>
-      <c r="H231" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H231" s="2">
+        <v>9.5830225538009088</v>
       </c>
       <c r="I231" s="2">
         <v>66.699200000000005</v>
@@ -10650,8 +10650,8 @@
       <c r="G232" s="2">
         <v>130.91946666666669</v>
       </c>
-      <c r="H232" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H232" s="2">
+        <v>9.6019922448101216</v>
       </c>
       <c r="I232" s="2">
         <v>67.323400000000007</v>
@@ -10694,8 +10694,8 @@
       <c r="G233" s="2">
         <v>131.72646666666665</v>
       </c>
-      <c r="H233" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H233" s="2">
+        <v>9.6050440053859614</v>
       </c>
       <c r="I233" s="2">
         <v>68.611699999999999</v>
@@ -10738,8 +10738,8 @@
       <c r="G234" s="2">
         <v>130.90536666666665</v>
       </c>
-      <c r="H234" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H234" s="2">
+        <v>9.4498853791327075</v>
       </c>
       <c r="I234" s="2">
         <v>68.712800000000001</v>
@@ -10782,8 +10782,8 @@
       <c r="G235" s="2">
         <v>132.47409999999999</v>
       </c>
-      <c r="H235" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H235" s="2">
+        <v>9.315041064099189</v>
       </c>
       <c r="I235" s="2">
         <v>69.847099999999998</v>
@@ -10826,8 +10826,8 @@
       <c r="G236" s="2">
         <v>132.81363333333334</v>
       </c>
-      <c r="H236" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H236" s="2">
+        <v>9.3925017342660624</v>
       </c>
       <c r="I236" s="2">
         <v>70.781199999999998</v>
@@ -10870,8 +10870,8 @@
       <c r="G237" s="2">
         <v>134.26813333333334</v>
       </c>
-      <c r="H237" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H237" s="2">
+        <v>9.4329326184392777</v>
       </c>
       <c r="I237" s="2">
         <v>71.366799999999998</v>
@@ -10914,8 +10914,8 @@
       <c r="G238" s="2">
         <v>136.17186666666666</v>
       </c>
-      <c r="H238" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H238" s="2">
+        <v>9.1820884451461566</v>
       </c>
       <c r="I238" s="2">
         <v>72.667500000000004</v>
@@ -10958,8 +10958,8 @@
       <c r="G239" s="2">
         <v>133.77359999999999</v>
       </c>
-      <c r="H239" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H239" s="2">
+        <v>9.1777645683907547</v>
       </c>
       <c r="I239" s="2">
         <v>72.466399999999993</v>
@@ -11002,8 +11002,8 @@
       <c r="G240" s="2">
         <v>132.29876666666667</v>
       </c>
-      <c r="H240" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H240" s="2">
+        <v>9.2636488887000112</v>
       </c>
       <c r="I240" s="2">
         <v>71.773600000000002</v>
@@ -11046,8 +11046,8 @@
       <c r="G241" s="2">
         <v>132.5213</v>
       </c>
-      <c r="H241" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H241" s="2">
+        <v>9.3607976989101527</v>
       </c>
       <c r="I241" s="2">
         <v>72.406700000000001</v>
@@ -11090,8 +11090,8 @@
       <c r="G242" s="2">
         <v>131.45426666666665</v>
       </c>
-      <c r="H242" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H242" s="2">
+        <v>9.5162661151138686</v>
       </c>
       <c r="I242" s="2">
         <v>71.059799999999996</v>
@@ -11134,8 +11134,8 @@
       <c r="G243" s="2">
         <v>133.34413333333333</v>
       </c>
-      <c r="H243" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H243" s="2">
+        <v>9.6431811256706386</v>
       </c>
       <c r="I243" s="2">
         <v>72.851799999999997</v>
@@ -11178,8 +11178,8 @@
       <c r="G244" s="2">
         <v>133.89313333333334</v>
       </c>
-      <c r="H244" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H244" s="2">
+        <v>9.7207802126238914</v>
       </c>
       <c r="I244" s="2">
         <v>73.448599999999999</v>
@@ -11222,8 +11222,8 @@
       <c r="G245" s="2">
         <v>131.24860000000001</v>
       </c>
-      <c r="H245" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H245" s="2">
+        <v>9.6741996683702052</v>
       </c>
       <c r="I245" s="2">
         <v>73.245099999999994</v>
@@ -11266,8 +11266,8 @@
       <c r="G246" s="2">
         <v>131.82646666666668</v>
       </c>
-      <c r="H246" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H246" s="2">
+        <v>9.8696441707347535</v>
       </c>
       <c r="I246" s="2">
         <v>73.316800000000001</v>
@@ -11310,8 +11310,8 @@
       <c r="G247" s="2">
         <v>131.22503333333333</v>
       </c>
-      <c r="H247" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H247" s="2">
+        <v>9.6155834549772496</v>
       </c>
       <c r="I247" s="2">
         <v>73.453199999999995</v>
@@ -11354,8 +11354,8 @@
       <c r="G248" s="2">
         <v>130.75360000000001</v>
       </c>
-      <c r="H248" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H248" s="2">
+        <v>9.6251671696149828</v>
       </c>
       <c r="I248" s="2">
         <v>73.671499999999995</v>
@@ -11398,8 +11398,8 @@
       <c r="G249" s="2">
         <v>131.48483333333334</v>
       </c>
-      <c r="H249" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H249" s="2">
+        <v>9.6930441251441248</v>
       </c>
       <c r="I249" s="2">
         <v>73.899900000000002</v>
@@ -11442,8 +11442,8 @@
       <c r="G250" s="2">
         <v>130.76079999999999</v>
       </c>
-      <c r="H250" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H250" s="2">
+        <v>9.8305644980476039</v>
       </c>
       <c r="I250" s="2">
         <v>73.582599999999999</v>
@@ -11486,8 +11486,8 @@
       <c r="G251" s="2">
         <v>131.47643333333335</v>
       </c>
-      <c r="H251" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H251" s="2">
+        <v>9.94</v>
       </c>
       <c r="I251" s="2">
         <v>74.327500000000001</v>
@@ -11530,8 +11530,8 @@
       <c r="G252" s="2">
         <v>131.36283333333333</v>
       </c>
-      <c r="H252" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H252" s="2">
+        <v>10.09</v>
       </c>
       <c r="I252" s="2">
         <v>74.547499999999999</v>
@@ -11574,8 +11574,8 @@
       <c r="G253" s="2">
         <v>131.20273333333333</v>
       </c>
-      <c r="H253" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H253" s="2">
+        <v>10.3</v>
       </c>
       <c r="I253" s="2">
         <v>74.325500000000005</v>
@@ -11618,8 +11618,8 @@
       <c r="G254" s="2">
         <v>131.15440000000001</v>
       </c>
-      <c r="H254" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H254" s="2">
+        <v>10.476000000000001</v>
       </c>
       <c r="I254" s="2">
         <v>74.117500000000007</v>
@@ -11662,8 +11662,8 @@
       <c r="G255" s="2">
         <v>130.6086</v>
       </c>
-      <c r="H255" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H255" s="2">
+        <v>10.576000000000001</v>
       </c>
       <c r="I255" s="2">
         <v>73.762799999999999</v>
@@ -11706,8 +11706,8 @@
       <c r="G256" s="2">
         <v>129.31723333333332</v>
       </c>
-      <c r="H256" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H256" s="2">
+        <v>10.555999999999999</v>
       </c>
       <c r="I256" s="2">
         <v>70.923100000000005</v>
@@ -11750,8 +11750,8 @@
       <c r="G257" s="2">
         <v>129.75370000000001</v>
       </c>
-      <c r="H257" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H257" s="2">
+        <v>10.476000000000001</v>
       </c>
       <c r="I257" s="2">
         <v>71.328699999999998</v>
@@ -11794,8 +11794,8 @@
       <c r="G258" s="2">
         <v>129.20246666666665</v>
       </c>
-      <c r="H258" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H258" s="2">
+        <v>10.677</v>
       </c>
       <c r="I258" s="2">
         <v>71.782499999999999</v>
@@ -11838,8 +11838,8 @@
       <c r="G259" s="2">
         <v>128.61600000000001</v>
       </c>
-      <c r="H259" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H259" s="2">
+        <v>10.919</v>
       </c>
       <c r="I259" s="2">
         <v>71.993099999999998</v>
@@ -11882,8 +11882,8 @@
       <c r="G260" s="2">
         <v>129.40700000000001</v>
       </c>
-      <c r="H260" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H260" s="2">
+        <v>10.766999999999999</v>
       </c>
       <c r="I260" s="2">
         <v>72.358199999999997</v>
@@ -11926,8 +11926,8 @@
       <c r="G261" s="2">
         <v>130.59513333333334</v>
       </c>
-      <c r="H261" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H261" s="2">
+        <v>10.941000000000001</v>
       </c>
       <c r="I261" s="2">
         <v>73.890799999999999</v>
@@ -11970,8 +11970,8 @@
       <c r="G262" s="2">
         <v>130.09903333333332</v>
       </c>
-      <c r="H262" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H262" s="2">
+        <v>10.951000000000001</v>
       </c>
       <c r="I262" s="2">
         <v>73.961399999999998</v>
@@ -12014,8 +12014,8 @@
       <c r="G263" s="2">
         <v>128.55526666666665</v>
       </c>
-      <c r="H263" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H263" s="2">
+        <v>10.941000000000001</v>
       </c>
       <c r="I263" s="2">
         <v>72.760999999999996</v>
@@ -12058,8 +12058,8 @@
       <c r="G264" s="2">
         <v>127.47316666666667</v>
       </c>
-      <c r="H264" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H264" s="2">
+        <v>11.042999999999999</v>
       </c>
       <c r="I264" s="2">
         <v>70.268500000000003</v>
@@ -12102,8 +12102,8 @@
       <c r="G265" s="2">
         <v>129.1165</v>
       </c>
-      <c r="H265" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H265" s="2">
+        <v>11.175000000000001</v>
       </c>
       <c r="I265" s="2">
         <v>71.613299999999995</v>
@@ -12146,8 +12146,8 @@
       <c r="G266" s="2">
         <v>128.36896666666667</v>
       </c>
-      <c r="H266" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H266" s="2">
+        <v>11.237</v>
       </c>
       <c r="I266" s="2">
         <v>71.6982</v>
@@ -12190,8 +12190,8 @@
       <c r="G267" s="2">
         <v>126.80476666666665</v>
       </c>
-      <c r="H267" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H267" s="2">
+        <v>11.340999999999999</v>
       </c>
       <c r="I267" s="2">
         <v>70.8155</v>
@@ -12234,8 +12234,8 @@
       <c r="G268" s="2">
         <v>125.77416666666666</v>
       </c>
-      <c r="H268" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H268" s="2">
+        <v>11.393000000000001</v>
       </c>
       <c r="I268" s="2">
         <v>69.963999999999999</v>
@@ -12278,8 +12278,8 @@
       <c r="G269" s="2">
         <v>122.96986666666668</v>
       </c>
-      <c r="H269" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H269" s="2">
+        <v>11.32</v>
       </c>
       <c r="I269" s="2">
         <v>67.381200000000007</v>
@@ -12322,8 +12322,8 @@
       <c r="G270" s="2">
         <v>121.75516666666668</v>
       </c>
-      <c r="H270" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H270" s="2">
+        <v>10.885</v>
       </c>
       <c r="I270" s="2">
         <v>65.987200000000001</v>
@@ -12366,8 +12366,8 @@
       <c r="G271" s="2">
         <v>121.60610000000001</v>
       </c>
-      <c r="H271" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H271" s="2">
+        <v>10.896000000000001</v>
       </c>
       <c r="I271" s="2">
         <v>65.546300000000002</v>
@@ -12410,8 +12410,8 @@
       <c r="G272" s="2">
         <v>120.68526666666666</v>
       </c>
-      <c r="H272" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H272" s="2">
+        <v>10.834</v>
       </c>
       <c r="I272" s="2">
         <v>64.536600000000007</v>
@@ -12454,8 +12454,8 @@
       <c r="G273" s="2">
         <v>124.52823333333333</v>
       </c>
-      <c r="H273" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H273" s="2">
+        <v>10.834</v>
       </c>
       <c r="I273" s="2">
         <v>66.868899999999996</v>
@@ -12498,8 +12498,8 @@
       <c r="G274" s="2">
         <v>121.92843333333333</v>
       </c>
-      <c r="H274" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H274" s="2">
+        <v>10.666</v>
       </c>
       <c r="I274" s="2">
         <v>64.991699999999994</v>
@@ -12542,8 +12542,8 @@
       <c r="G275" s="2">
         <v>119.06683333333335</v>
       </c>
-      <c r="H275" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H275" s="2">
+        <v>10.34</v>
       </c>
       <c r="I275" s="2">
         <v>63.910800000000002</v>
@@ -12586,8 +12586,8 @@
       <c r="G276" s="2">
         <v>120.05546666666667</v>
       </c>
-      <c r="H276" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H276" s="2">
+        <v>10.119</v>
       </c>
       <c r="I276" s="2">
         <v>64.749899999999997</v>
@@ -12630,8 +12630,8 @@
       <c r="G277" s="2">
         <v>119.67529999999999</v>
       </c>
-      <c r="H277" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H277" s="2">
+        <v>10.266999999999999</v>
       </c>
       <c r="I277" s="2">
         <v>65.6601</v>
@@ -12674,8 +12674,8 @@
       <c r="G278" s="2">
         <v>116.54123333333332</v>
       </c>
-      <c r="H278" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H278" s="2">
+        <v>10.58</v>
       </c>
       <c r="I278" s="2">
         <v>64.209500000000006</v>
@@ -12718,8 +12718,8 @@
       <c r="G279" s="2">
         <v>118.28179999999999</v>
       </c>
-      <c r="H279" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H279" s="2">
+        <v>10.868</v>
       </c>
       <c r="I279" s="2">
         <v>66.072500000000005</v>
@@ -12762,8 +12762,8 @@
       <c r="G280" s="2">
         <v>117.24953333333333</v>
       </c>
-      <c r="H280" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H280" s="2">
+        <v>10.612</v>
       </c>
       <c r="I280" s="2">
         <v>65.020099999999999</v>
@@ -12806,8 +12806,8 @@
       <c r="G281" s="2">
         <v>119.13773333333332</v>
       </c>
-      <c r="H281" s="2" t="e">
-        <v>#N/A</v>
+      <c r="H281" s="2">
+        <v>10.760999999999999</v>
       </c>
       <c r="I281" s="2">
         <v>67.224400000000003</v>

</xml_diff>